<commit_message>
Minor updates to pd.rolling.aggregates files
</commit_message>
<xml_diff>
--- a/pd.rolling.aggregate/excel-lambda-pd.rolling.aggregate.xlsx
+++ b/pd.rolling.aggregate/excel-lambda-pd.rolling.aggregate.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owen.price\Documents\Me\Drive\Blog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owen.price\Documents\Me\Drive\Blog\pandas-lambdas\pd.rolling.aggregate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA54C932-BEBC-4048-9D58-9D58F626A63D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFDBAB9C-9074-42D5-B689-1CA42D949907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15510" activeTab="2" xr2:uid="{DCA575A9-AF13-4812-ABF9-9F6A4A01F50D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DCA575A9-AF13-4812-ABF9-9F6A4A01F50D}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="5" r:id="rId1"/>
@@ -18,13 +18,9 @@
     <sheet name="3" sheetId="6" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_agg">#REF!</definedName>
-    <definedName name="_w">#REF!</definedName>
     <definedName name="aggs" comment="List of aggregate functions supported by pd.rolling.aggregate">'2'!$G$2:$G$16</definedName>
-    <definedName name="pd.qcut">_xlfn.LAMBDA(_xlpm.x,_xlpm.q,_xlop.labels,_xlop.return,   _xlfn.LET(     _xlpm._s,_xlfn.SEQUENCE(ROWS(_xlpm.x)),     _xlpm._x,_xlfn._xlws.SORT(CHOOSE({1,2},_xlpm.x,_xlpm._s),1,1),     _xlpm._xval,INDEX(_xlpm._x,,1),     _xlpm._xord,INDEX(_xlpm._x,,2),     _xlpm._q,_xlpm.q,     _xlpm._lbl,IF(_xlfn.ISOMITTED(_xlpm.labels),_xlfn.SEQUENCE(_xlpm._q),_xlpm.labels),     _xlpm._ret,IF(_xlfn.ISOMITTED(_xlpm.return),"row labels",_xlpm.return),     _xlpm._rnk,_xlfn.SCAN(0,_xlpm._s,           _xlfn.LAMBDA(_xlpm.a,_xlpm.b,             _xlfn.IFS(               _xlpm.b=1,1,               INDEX(_xlpm._xval,_xlpm.b-1,1)=INDEX(_xlpm._xval,_xlpm.b,1),_xlpm.a,               TRUE,_xlpm.a+1             )           )          ),     _xlpm._mxrank,MAX(_xlpm._rnk),     _xlpm._brk,_xlpm._mxrank/_xlpm._q,     _xlpm._quo,QUOTIENT(_xlpm._rnk-1,_xlpm._brk),     _xlpm._xlbl,IF(             _xlpm._q&lt;&gt;ROWS(_xlpm._lbl),             "Label array is not the same size as q",             _xlfn.SORTBY(INDEX(_xlpm._lbl,_xlpm._quo+1),_xlpm._xord,1)           ),     _xlpm._u_quo,_xlfn.UNIQUE(_xlpm._quo),     _xlpm._maxs,_xlfn.MAP(_xlpm._u_quo,_xlfn.LAMBDA(_xlpm.u,MAX(_xlfn._xlws.FILTER(_xlpm._xval,_xlpm._quo=_xlpm.u)))),     _xlpm._actual_mins,_xlfn.MAP(_xlpm._u_quo,_xlfn.LAMBDA(_xlpm.u,MIN(_xlfn._xlws.FILTER(_xlpm._xval,_xlpm._quo=_xlpm.u)))),     _xlpm._freqs,_xlfn.MAP(_xlpm._u_quo,_xlfn.LAMBDA(_xlpm.u,ROWS(_xlfn._xlws.FILTER(_xlpm._xval,_xlpm._quo=_xlpm.u)))),     _xlpm._global_min,INDEX(_xlpm._actual_mins,1,1),     _xlpm._mins,_xlfn.MAKEARRAY(             _xlpm._q,             1,             _xlfn.LAMBDA(_xlpm.r,_xlpm.c,               IF(                 _xlpm.r=1,                 _xlpm._global_min-_xlpm._global_min*0.01%,                 INDEX(_xlpm._maxs,_xlpm.r-1,1)               )             )           ),     _xlpm._grps,CHOOSE(             {1,2,3,4,5,6},             _xlpm._lbl,             "("&amp;_xlpm._mins&amp;","&amp;_xlpm._maxs&amp;"]",             _xlpm._mins,             _xlpm._maxs,             "["&amp;_xlpm._actual_mins&amp;","&amp;_xlpm._maxs&amp;"]",             _xlpm._freqs           ),     _xlpm._h,{"group","range","range_low","range_high","actual_range","frequencies"},     _xlpm._hgrps,_xlfn.MAKEARRAY(             _xlpm._q+1,             6,             _xlfn.LAMBDA(_xlpm.r,_xlpm.c,               IF(                 _xlpm.r=1,                 INDEX(_xlpm._h,1,_xlpm.c),                 INDEX(_xlpm._grps,_xlpm.r-1,_xlpm.c)               )             )            ),     IF(_xlpm._ret="row labels",_xlpm._xlbl,_xlpm._hgrps)   ) )</definedName>
-    <definedName name="pd.rolling.aggregate">_xlfn.LAMBDA(_xlpm.x,_xlpm.window,_xlpm.agg,   _xlfn.LET(     _xlpm._x,_xlpm.x,     _xlpm._w,_xlpm.window,     _xlpm._agg,_xlpm.agg,     _xlpm._aggs,{"average";"count";"counta";"max";"min";"product";"stdev.s";"stdev.p";"sum";"var.s";"var.p";"median";"mode.sngl";"kurt";"skew";"sem"},     _xlpm._thk,_xlfn.LAMBDA(_xlpm.x,_xlfn.LAMBDA(_xlpm.x)),     _xlpm._fn_aggs,_xlfn.MAKEARRAY(ROWS(_xlpm._aggs),1,               _xlfn.LAMBDA(_xlpm.r,_xlpm.c,                 CHOOSE(                   _xlpm.r,                   _xlpm._thk(_xlfn.LAMBDA(_xlpm.x,AVERAGE(_xlpm.x))),                   _xlpm._thk(_xlfn.LAMBDA(_xlpm.x,COUNT(_xlpm.x))),                   _xlpm._thk(_xlfn.LAMBDA(_xlpm.x,COUNTA(_xlpm.x))),                   _xlpm._thk(_xlfn.LAMBDA(_xlpm.x,MAX(_xlpm.x))),                   _xlpm._thk(_xlfn.LAMBDA(_xlpm.x,MIN(_xlpm.x))),                   _xlpm._thk(_xlfn.LAMBDA(_xlpm.x,PRODUCT(_xlpm.x))),                   _xlpm._thk(_xlfn.LAMBDA(_xlpm.x,_xlfn.STDEV.S(_xlpm.x))),                   _xlpm._thk(_xlfn.LAMBDA(_xlpm.x,_xlfn.STDEV.P(_xlpm.x))),                   _xlpm._thk(_xlfn.LAMBDA(_xlpm.x,SUM(_xlpm.x))),                   _xlpm._thk(_xlfn.LAMBDA(_xlpm.x,_xlfn.VAR.S(_xlpm.x))),                   _xlpm._thk(_xlfn.LAMBDA(_xlpm.x,_xlfn.VAR.P(_xlpm.x))),                   _xlpm._thk(_xlfn.LAMBDA(_xlpm.x,MEDIAN(_xlpm.x))),                   _xlpm._thk(_xlfn.LAMBDA(_xlpm.x,_xlfn.MODE.SNGL(_xlpm.x))),                   _xlpm._thk(_xlfn.LAMBDA(_xlpm.x,KURT(_xlpm.x))),                   _xlpm._thk(_xlfn.LAMBDA(_xlpm.x,SKEW(_xlpm.x))),                   _xlpm._thk(_xlfn.LAMBDA(_xlpm.x,_xlfn.STDEV.S(_xlpm.x)/SQRT(_xlpm._w)))                 )               )              ),     _xlpm._fn,_xlfn.XLOOKUP(_xlpm._agg,_xlpm._aggs,_xlpm._fn_aggs),     _xlpm._i,_xlfn.SEQUENCE(ROWS(_xlpm.x)),     _xlpm._s,_xlfn.SCAN(0,_xlpm._i,         _xlfn.LAMBDA(_xlpm.a,_xlpm.b,           IF(             _xlpm.b&lt;_xlpm._w,             NA(),             _xlpm._thk(               _xlfn.MAKEARRAY(_xlpm._w,1,                 _xlfn.LAMBDA(_xlpm.r,_xlpm.c,                   INDEX(_xlpm._x,_xlpm.b-_xlpm._w+_xlpm.r)                 )               )             )           )         )        ),    _xlpm._out,_xlfn.SCAN(0,_xlpm._i,_xlfn.LAMBDA(_xlpm.a,_xlpm.b,_xlpm._fn()(INDEX(_xlpm._s,_xlpm.b,1)()))),    _xlpm._out   ) )</definedName>
-    <definedName name="pd.rolling.aggregates">_xlfn.LAMBDA(_xlpm.x,_xlpm.windows,_xlpm.aggs,   _xlfn.LET(     _xlpm._tr,_xlfn.LAMBDA(_xlpm.arr,_xlfn.LET(_xlpm.x,_xlfn._xlws.FILTER(_xlpm.arr,_xlpm.arr&lt;&gt;""),IF(ROWS(_xlpm.x)=1,TRANSPOSE(_xlpm.x),_xlpm.x))),     _xlpm._a,_xlpm._tr(_xlpm.aggs),     _xlpm._w,_xlpm._tr(_xlpm.windows),     _xlpm._resize,ROWS(_xlpm._a)&lt;&gt;ROWS(_xlpm._w),     _xlpm._rs,_xlfn.LAMBDA(_xlpm.arr,_xlpm.resize_to,_xlfn.MAKEARRAY(_xlpm.resize_to,1,_xlfn.LAMBDA(_xlpm.r,_xlpm.c,IF(_xlpm.r&lt;=ROWS(_xlpm.arr),INDEX(_xlpm.arr,_xlpm.r,1),INDEX(_xlpm.arr,ROWS(_xlpm.arr),1))))),     _xlpm._ms,MAX(ROWS(_xlpm._a),ROWS(_xlpm._w)),     _xlpm._ar,IF(_xlpm._resize,_xlpm._rs(_xlpm._a,_xlpm._ms),_xlpm._a),     _xlpm._wr,IF(_xlpm._resize,_xlpm._rs(_xlpm._w,_xlpm._ms),_xlpm._w),     _xlpm._out,     _xlfn.MAKEARRAY(       ROWS(_xlpm.x),       _xlpm._ms,       _xlfn.LAMBDA(_xlpm.r,_xlpm.c,         INDEX(pd.rolling.aggregate(_xlpm.x,INDEX(_xlpm._wr,_xlpm.c,1),INDEX(_xlpm._ar,_xlpm.c,1)),_xlpm.r,1)       )     ),     _xlpm._out   ) )</definedName>
-    <definedName name="test.pd.qcut">_xlfn.LAMBDA(_xlpm.x,_xlpm.q,_xlop.labels,_xlop.return,   _xlfn.LET(     _xlpm._s,_xlfn.SEQUENCE(ROWS(_xlpm.x)),     _xlpm._x,_xlfn._xlws.SORT(CHOOSE({1,2},_xlpm.x,_xlpm._s),1,1),     _xlpm._xval,INDEX(_xlpm._x,,1),     _xlpm._xord,INDEX(_xlpm._x,,2),     _xlpm._q,_xlpm.q,     _xlpm._lbl,IF(_xlfn.ISOMITTED(_xlpm.labels),_xlfn.SEQUENCE(_xlpm._q),_xlpm.labels),     _xlpm._ret,IF(_xlfn.ISOMITTED(_xlpm.return),"row labels",_xlpm.return),     _xlpm._rnk,_xlfn.SCAN(0,_xlpm._s,           _xlfn.LAMBDA(_xlpm.a,_xlpm.b,             _xlfn.IFS(               _xlpm.b=1,1,               INDEX(_xlpm._xval,_xlpm.b-1,1)=INDEX(_xlpm._xval,_xlpm.b,1),_xlpm.a,               TRUE,_xlpm.a+1             )           )          ),     _xlpm._mxrank,MAX(_xlpm._rnk),     _xlpm._brk,_xlpm._mxrank/_xlpm._q,     _xlpm._quo,QUOTIENT(_xlpm._rnk-1,_xlpm._brk),     _xlpm._xlbl,IF(             _xlpm._q&lt;&gt;ROWS(_xlpm._lbl),             "Label array is not the same size as q",             _xlfn.SORTBY(INDEX(_xlpm._lbl,_xlpm._quo+1),_xlpm._xord,1)           ),     _xlpm._u_quo,_xlfn.UNIQUE(_xlpm._quo),     _xlpm._maxs,_xlfn.MAP(_xlpm._u_quo,_xlfn.LAMBDA(_xlpm.u,MAX(_xlfn._xlws.FILTER(_xlpm._xval,_xlpm._quo=_xlpm.u)))),     _xlpm._actual_mins,_xlfn.MAP(_xlpm._u_quo,_xlfn.LAMBDA(_xlpm.u,MIN(_xlfn._xlws.FILTER(_xlpm._xval,_xlpm._quo=_xlpm.u)))),     _xlpm._freqs,_xlfn.MAP(_xlpm._u_quo,_xlfn.LAMBDA(_xlpm.u,ROWS(_xlfn._xlws.FILTER(_xlpm._xval,_xlpm._quo=_xlpm.u)))),     _xlpm._global_min,INDEX(_xlpm._actual_mins,1,1),     _xlpm._mins,_xlfn.MAKEARRAY(             _xlpm._q,             1,             _xlfn.LAMBDA(_xlpm.r,_xlpm.c,               IF(                 _xlpm.r=1,                 _xlpm._global_min-_xlpm._global_min*0.01%,                 INDEX(_xlpm._maxs,_xlpm.r-1,1)               )             )           ),     _xlpm._grps,CHOOSE(             {1,2,3,4,5,6},             _xlpm._lbl,             "("&amp;_xlpm._mins&amp;","&amp;_xlpm._maxs&amp;"]",             _xlpm._mins,             _xlpm._maxs,             "["&amp;_xlpm._actual_mins&amp;","&amp;_xlpm._maxs&amp;"]",             _xlpm._freqs           ),     _xlpm._h,{"group","range","range_low","range_high","actual_range","frequencies"},     _xlpm._hgrps,_xlfn.MAKEARRAY(             _xlpm._q+1,             6,             _xlfn.LAMBDA(_xlpm.r,_xlpm.c,               IF(                 _xlpm.r=1,                 INDEX(_xlpm._h,1,_xlpm.c),                 INDEX(_xlpm._grps,_xlpm.r-1,_xlpm.c)               )             )            ),     _xlpm._quo   ) )</definedName>
+    <definedName name="pd.rolling.aggregate" comment="Calculates the aggregate [agg] over rolling windows of size [window]">_xlfn.LAMBDA(_xlpm.x,_xlpm.window,_xlpm.agg,   _xlfn.LET(     _xlpm._x,_xlpm.x,     _xlpm._w,_xlpm.window,     _xlpm._agg,_xlpm.agg,     _xlpm._aggs,{"average";"count";"counta";"max";"min";"product";"stdev.s";"stdev.p";"sum";"var.s";"var.p";"median";"mode.sngl";"kurt";"skew";"sem"},     _xlpm._thk,_xlfn.LAMBDA(_xlpm.x,_xlfn.LAMBDA(_xlpm.x)),     _xlpm._fn_aggs,_xlfn.MAKEARRAY(ROWS(_xlpm._aggs),1,               _xlfn.LAMBDA(_xlpm.r,_xlpm.c,                 CHOOSE(                   _xlpm.r,                   _xlpm._thk(_xlfn.LAMBDA(_xlpm.x,AVERAGE(_xlpm.x))),                   _xlpm._thk(_xlfn.LAMBDA(_xlpm.x,COUNT(_xlpm.x))),                   _xlpm._thk(_xlfn.LAMBDA(_xlpm.x,COUNTA(_xlpm.x))),                   _xlpm._thk(_xlfn.LAMBDA(_xlpm.x,MAX(_xlpm.x))),                   _xlpm._thk(_xlfn.LAMBDA(_xlpm.x,MIN(_xlpm.x))),                   _xlpm._thk(_xlfn.LAMBDA(_xlpm.x,PRODUCT(_xlpm.x))),                   _xlpm._thk(_xlfn.LAMBDA(_xlpm.x,_xlfn.STDEV.S(_xlpm.x))),                   _xlpm._thk(_xlfn.LAMBDA(_xlpm.x,_xlfn.STDEV.P(_xlpm.x))),                   _xlpm._thk(_xlfn.LAMBDA(_xlpm.x,SUM(_xlpm.x))),                   _xlpm._thk(_xlfn.LAMBDA(_xlpm.x,_xlfn.VAR.S(_xlpm.x))),                   _xlpm._thk(_xlfn.LAMBDA(_xlpm.x,_xlfn.VAR.P(_xlpm.x))),                   _xlpm._thk(_xlfn.LAMBDA(_xlpm.x,MEDIAN(_xlpm.x))),                   _xlpm._thk(_xlfn.LAMBDA(_xlpm.x,_xlfn.MODE.SNGL(_xlpm.x))),                   _xlpm._thk(_xlfn.LAMBDA(_xlpm.x,KURT(_xlpm.x))),                   _xlpm._thk(_xlfn.LAMBDA(_xlpm.x,SKEW(_xlpm.x))),                   _xlpm._thk(_xlfn.LAMBDA(_xlpm.x,_xlfn.STDEV.S(_xlpm.x)/SQRT(_xlpm._w)))                 )               )              ),     _xlpm._fn,_xlfn.XLOOKUP(_xlpm._agg,_xlpm._aggs,_xlpm._fn_aggs),     _xlpm._i,_xlfn.SEQUENCE(ROWS(_xlpm.x)),     _xlpm._s,_xlfn.SCAN(0,_xlpm._i,         _xlfn.LAMBDA(_xlpm.a,_xlpm.b,           IF(             _xlpm.b&lt;_xlpm._w,             NA(),             _xlpm._thk(               _xlfn.MAKEARRAY(_xlpm._w,1,                 _xlfn.LAMBDA(_xlpm.r,_xlpm.c,                   INDEX(_xlpm._x,_xlpm.b-_xlpm._w+_xlpm.r)                 )               )             )           )         )        ),    _xlpm._out,_xlfn.SCAN(0,_xlpm._i,_xlfn.LAMBDA(_xlpm.a,_xlpm.b,_xlpm._fn()(INDEX(_xlpm._s,_xlpm.b,1)()))),    _xlpm._out   ) )</definedName>
+    <definedName name="pd.rolling.aggregates" comment="Calculates the set of aggregates [aggs] over the aligned set of rolling windows of size [windows]">_xlfn.LAMBDA(_xlpm.x,_xlpm.windows,_xlpm.aggs,   _xlfn.LET(     _xlpm._tr,_xlfn.LAMBDA(_xlpm.arr,_xlfn.LET(_xlpm.x,_xlfn._xlws.FILTER(_xlpm.arr,_xlpm.arr&lt;&gt;""),IF(ROWS(_xlpm.x)=1,TRANSPOSE(_xlpm.x),_xlpm.x))),     _xlpm._a,_xlpm._tr(_xlpm.aggs),     _xlpm._w,_xlpm._tr(_xlpm.windows),     _xlpm._resize,ROWS(_xlpm._a)&lt;&gt;ROWS(_xlpm._w),     _xlpm._rs,_xlfn.LAMBDA(_xlpm.arr,_xlpm.resize_to,_xlfn.MAKEARRAY(_xlpm.resize_to,1,_xlfn.LAMBDA(_xlpm.r,_xlpm.c,IF(_xlpm.r&lt;=ROWS(_xlpm.arr),INDEX(_xlpm.arr,_xlpm.r,1),INDEX(_xlpm.arr,ROWS(_xlpm.arr),1))))),     _xlpm._ms,MAX(ROWS(_xlpm._a),ROWS(_xlpm._w)),     _xlpm._ar,IF(_xlpm._resize,_xlpm._rs(_xlpm._a,_xlpm._ms),_xlpm._a),     _xlpm._wr,IF(_xlpm._resize,_xlpm._rs(_xlpm._w,_xlpm._ms),_xlpm._w),     _xlpm._out,     _xlfn.MAKEARRAY(       ROWS(_xlpm.x),       _xlpm._ms,       _xlfn.LAMBDA(_xlpm.r,_xlpm.c,         INDEX(pd.rolling.aggregate(_xlpm.x,INDEX(_xlpm._wr,_xlpm.c,1),INDEX(_xlpm._ar,_xlpm.c,1)),_xlpm.r,1)       )     ),     _xlpm._out   ) )</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1469,7 +1465,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>aggs will be etended such that it becomes:</a:t>
+            <a:t>aggs will be extended such that it becomes:</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1830,10 +1826,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C59E16A-7D8F-4637-9C37-8A31CFB0AAF9}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:P38"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="T27" sqref="T27"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1965,7 +1962,7 @@
         <v>=SUM(OFFSET(B7,-2,0,3))</v>
       </c>
       <c r="L7" s="8">
-        <f>SUM(B5:B7)</f>
+        <f t="shared" ref="L7:L17" si="0">SUM(B5:B7)</f>
         <v>195</v>
       </c>
       <c r="M7" s="8" t="str">
@@ -1973,7 +1970,7 @@
         <v>=SUM(B5:B7)</v>
       </c>
       <c r="O7" s="16">
-        <f>_xlfn.AGGREGATE(9,4,B5:B7)</f>
+        <f t="shared" ref="O7:O17" si="1">_xlfn.AGGREGATE(9,4,B5:B7)</f>
         <v>195</v>
       </c>
       <c r="P7" s="16" t="str">
@@ -1986,11 +1983,11 @@
         <v>72</v>
       </c>
       <c r="C8" s="9">
-        <f t="shared" ref="C8:C17" si="0">B8+B7+B6</f>
+        <f t="shared" ref="C8:C17" si="2">B8+B7+B6</f>
         <v>214</v>
       </c>
       <c r="D8" s="5" t="str">
-        <f t="shared" ref="D8:D17" ca="1" si="1">_xlfn.FORMULATEXT(C8)</f>
+        <f t="shared" ref="D8:D17" ca="1" si="3">_xlfn.FORMULATEXT(C8)</f>
         <v>=B8+B7+B6</v>
       </c>
       <c r="F8" s="9">
@@ -1998,27 +1995,27 @@
       </c>
       <c r="G8" s="5"/>
       <c r="I8" s="4">
-        <f t="shared" ref="I8:I17" ca="1" si="2">SUM(OFFSET(B8,-2,0,3))</f>
+        <f t="shared" ref="I8:I17" ca="1" si="4">SUM(OFFSET(B8,-2,0,3))</f>
         <v>214</v>
       </c>
       <c r="J8" s="4" t="str">
-        <f t="shared" ref="J8:J17" ca="1" si="3">_xlfn.FORMULATEXT(I8)</f>
+        <f t="shared" ref="J8:J17" ca="1" si="5">_xlfn.FORMULATEXT(I8)</f>
         <v>=SUM(OFFSET(B8,-2,0,3))</v>
       </c>
       <c r="L8" s="8">
-        <f>SUM(B6:B8)</f>
+        <f t="shared" si="0"/>
         <v>214</v>
       </c>
       <c r="M8" s="8" t="str">
-        <f t="shared" ref="M8:M17" ca="1" si="4">_xlfn.FORMULATEXT(L8)</f>
+        <f t="shared" ref="M8:M17" ca="1" si="6">_xlfn.FORMULATEXT(L8)</f>
         <v>=SUM(B6:B8)</v>
       </c>
       <c r="O8" s="16">
-        <f>_xlfn.AGGREGATE(9,4,B6:B8)</f>
+        <f t="shared" si="1"/>
         <v>214</v>
       </c>
       <c r="P8" s="16" t="str">
-        <f t="shared" ref="P8:P17" ca="1" si="5">_xlfn.FORMULATEXT(O8)</f>
+        <f t="shared" ref="P8:P17" ca="1" si="7">_xlfn.FORMULATEXT(O8)</f>
         <v>=AGGREGATE(9,4,B6:B8)</v>
       </c>
     </row>
@@ -2027,39 +2024,39 @@
         <v>80</v>
       </c>
       <c r="C9" s="9">
+        <f t="shared" si="2"/>
+        <v>201</v>
+      </c>
+      <c r="D9" s="5" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>=B9+B8+B7</v>
+      </c>
+      <c r="F9" s="9">
+        <v>201</v>
+      </c>
+      <c r="G9" s="5"/>
+      <c r="I9" s="4">
+        <f t="shared" ca="1" si="4"/>
+        <v>201</v>
+      </c>
+      <c r="J9" s="4" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>=SUM(OFFSET(B9,-2,0,3))</v>
+      </c>
+      <c r="L9" s="8">
         <f t="shared" si="0"/>
         <v>201</v>
       </c>
-      <c r="D9" s="5" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>=B9+B8+B7</v>
-      </c>
-      <c r="F9" s="9">
+      <c r="M9" s="8" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>=SUM(B7:B9)</v>
+      </c>
+      <c r="O9" s="16">
+        <f t="shared" si="1"/>
         <v>201</v>
       </c>
-      <c r="G9" s="5"/>
-      <c r="I9" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>201</v>
-      </c>
-      <c r="J9" s="4" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>=SUM(OFFSET(B9,-2,0,3))</v>
-      </c>
-      <c r="L9" s="8">
-        <f>SUM(B7:B9)</f>
-        <v>201</v>
-      </c>
-      <c r="M9" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>=SUM(B7:B9)</v>
-      </c>
-      <c r="O9" s="16">
-        <f>_xlfn.AGGREGATE(9,4,B7:B9)</f>
-        <v>201</v>
-      </c>
       <c r="P9" s="16" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="7"/>
         <v>=AGGREGATE(9,4,B7:B9)</v>
       </c>
     </row>
@@ -2068,39 +2065,39 @@
         <v>79</v>
       </c>
       <c r="C10" s="9">
+        <f t="shared" si="2"/>
+        <v>231</v>
+      </c>
+      <c r="D10" s="5" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>=B10+B9+B8</v>
+      </c>
+      <c r="F10" s="9">
+        <v>231</v>
+      </c>
+      <c r="G10" s="5"/>
+      <c r="I10" s="4">
+        <f t="shared" ca="1" si="4"/>
+        <v>231</v>
+      </c>
+      <c r="J10" s="4" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>=SUM(OFFSET(B10,-2,0,3))</v>
+      </c>
+      <c r="L10" s="8">
         <f t="shared" si="0"/>
         <v>231</v>
       </c>
-      <c r="D10" s="5" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>=B10+B9+B8</v>
-      </c>
-      <c r="F10" s="9">
+      <c r="M10" s="8" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>=SUM(B8:B10)</v>
+      </c>
+      <c r="O10" s="16">
+        <f t="shared" si="1"/>
         <v>231</v>
       </c>
-      <c r="G10" s="5"/>
-      <c r="I10" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>231</v>
-      </c>
-      <c r="J10" s="4" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>=SUM(OFFSET(B10,-2,0,3))</v>
-      </c>
-      <c r="L10" s="8">
-        <f>SUM(B8:B10)</f>
-        <v>231</v>
-      </c>
-      <c r="M10" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>=SUM(B8:B10)</v>
-      </c>
-      <c r="O10" s="16">
-        <f>_xlfn.AGGREGATE(9,4,B8:B10)</f>
-        <v>231</v>
-      </c>
       <c r="P10" s="16" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="7"/>
         <v>=AGGREGATE(9,4,B8:B10)</v>
       </c>
     </row>
@@ -2109,39 +2106,39 @@
         <v>52</v>
       </c>
       <c r="C11" s="9">
+        <f t="shared" si="2"/>
+        <v>211</v>
+      </c>
+      <c r="D11" s="5" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>=B11+B10+B9</v>
+      </c>
+      <c r="F11" s="9">
+        <v>211</v>
+      </c>
+      <c r="G11" s="5"/>
+      <c r="I11" s="4">
+        <f t="shared" ca="1" si="4"/>
+        <v>211</v>
+      </c>
+      <c r="J11" s="4" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>=SUM(OFFSET(B11,-2,0,3))</v>
+      </c>
+      <c r="L11" s="8">
         <f t="shared" si="0"/>
         <v>211</v>
       </c>
-      <c r="D11" s="5" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>=B11+B10+B9</v>
-      </c>
-      <c r="F11" s="9">
+      <c r="M11" s="8" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>=SUM(B9:B11)</v>
+      </c>
+      <c r="O11" s="16">
+        <f t="shared" si="1"/>
         <v>211</v>
       </c>
-      <c r="G11" s="5"/>
-      <c r="I11" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>211</v>
-      </c>
-      <c r="J11" s="4" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>=SUM(OFFSET(B11,-2,0,3))</v>
-      </c>
-      <c r="L11" s="8">
-        <f>SUM(B9:B11)</f>
-        <v>211</v>
-      </c>
-      <c r="M11" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>=SUM(B9:B11)</v>
-      </c>
-      <c r="O11" s="16">
-        <f>_xlfn.AGGREGATE(9,4,B9:B11)</f>
-        <v>211</v>
-      </c>
       <c r="P11" s="16" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="7"/>
         <v>=AGGREGATE(9,4,B9:B11)</v>
       </c>
     </row>
@@ -2150,39 +2147,39 @@
         <v>46</v>
       </c>
       <c r="C12" s="9">
+        <f t="shared" si="2"/>
+        <v>177</v>
+      </c>
+      <c r="D12" s="5" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>=B12+B11+B10</v>
+      </c>
+      <c r="F12" s="9">
+        <v>177</v>
+      </c>
+      <c r="G12" s="5"/>
+      <c r="I12" s="4">
+        <f t="shared" ca="1" si="4"/>
+        <v>177</v>
+      </c>
+      <c r="J12" s="4" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>=SUM(OFFSET(B12,-2,0,3))</v>
+      </c>
+      <c r="L12" s="8">
         <f t="shared" si="0"/>
         <v>177</v>
       </c>
-      <c r="D12" s="5" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>=B12+B11+B10</v>
-      </c>
-      <c r="F12" s="9">
+      <c r="M12" s="8" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>=SUM(B10:B12)</v>
+      </c>
+      <c r="O12" s="16">
+        <f t="shared" si="1"/>
         <v>177</v>
       </c>
-      <c r="G12" s="5"/>
-      <c r="I12" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>177</v>
-      </c>
-      <c r="J12" s="4" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>=SUM(OFFSET(B12,-2,0,3))</v>
-      </c>
-      <c r="L12" s="8">
-        <f>SUM(B10:B12)</f>
-        <v>177</v>
-      </c>
-      <c r="M12" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>=SUM(B10:B12)</v>
-      </c>
-      <c r="O12" s="16">
-        <f>_xlfn.AGGREGATE(9,4,B10:B12)</f>
-        <v>177</v>
-      </c>
       <c r="P12" s="16" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="7"/>
         <v>=AGGREGATE(9,4,B10:B12)</v>
       </c>
     </row>
@@ -2191,39 +2188,39 @@
         <v>86</v>
       </c>
       <c r="C13" s="9">
+        <f t="shared" si="2"/>
+        <v>184</v>
+      </c>
+      <c r="D13" s="5" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>=B13+B12+B11</v>
+      </c>
+      <c r="F13" s="9">
+        <v>184</v>
+      </c>
+      <c r="G13" s="5"/>
+      <c r="I13" s="4">
+        <f t="shared" ca="1" si="4"/>
+        <v>184</v>
+      </c>
+      <c r="J13" s="4" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>=SUM(OFFSET(B13,-2,0,3))</v>
+      </c>
+      <c r="L13" s="8">
         <f t="shared" si="0"/>
         <v>184</v>
       </c>
-      <c r="D13" s="5" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>=B13+B12+B11</v>
-      </c>
-      <c r="F13" s="9">
+      <c r="M13" s="8" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>=SUM(B11:B13)</v>
+      </c>
+      <c r="O13" s="16">
+        <f t="shared" si="1"/>
         <v>184</v>
       </c>
-      <c r="G13" s="5"/>
-      <c r="I13" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>184</v>
-      </c>
-      <c r="J13" s="4" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>=SUM(OFFSET(B13,-2,0,3))</v>
-      </c>
-      <c r="L13" s="8">
-        <f>SUM(B11:B13)</f>
-        <v>184</v>
-      </c>
-      <c r="M13" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>=SUM(B11:B13)</v>
-      </c>
-      <c r="O13" s="16">
-        <f>_xlfn.AGGREGATE(9,4,B11:B13)</f>
-        <v>184</v>
-      </c>
       <c r="P13" s="16" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="7"/>
         <v>=AGGREGATE(9,4,B11:B13)</v>
       </c>
     </row>
@@ -2232,39 +2229,39 @@
         <v>26</v>
       </c>
       <c r="C14" s="9">
+        <f t="shared" si="2"/>
+        <v>158</v>
+      </c>
+      <c r="D14" s="5" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>=B14+B13+B12</v>
+      </c>
+      <c r="F14" s="9">
+        <v>158</v>
+      </c>
+      <c r="G14" s="5"/>
+      <c r="I14" s="4">
+        <f t="shared" ca="1" si="4"/>
+        <v>158</v>
+      </c>
+      <c r="J14" s="4" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>=SUM(OFFSET(B14,-2,0,3))</v>
+      </c>
+      <c r="L14" s="8">
         <f t="shared" si="0"/>
         <v>158</v>
       </c>
-      <c r="D14" s="5" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>=B14+B13+B12</v>
-      </c>
-      <c r="F14" s="9">
+      <c r="M14" s="8" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>=SUM(B12:B14)</v>
+      </c>
+      <c r="O14" s="16">
+        <f t="shared" si="1"/>
         <v>158</v>
       </c>
-      <c r="G14" s="5"/>
-      <c r="I14" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>158</v>
-      </c>
-      <c r="J14" s="4" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>=SUM(OFFSET(B14,-2,0,3))</v>
-      </c>
-      <c r="L14" s="8">
-        <f>SUM(B12:B14)</f>
-        <v>158</v>
-      </c>
-      <c r="M14" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>=SUM(B12:B14)</v>
-      </c>
-      <c r="O14" s="16">
-        <f>_xlfn.AGGREGATE(9,4,B12:B14)</f>
-        <v>158</v>
-      </c>
       <c r="P14" s="16" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="7"/>
         <v>=AGGREGATE(9,4,B12:B14)</v>
       </c>
     </row>
@@ -2273,39 +2270,39 @@
         <v>49</v>
       </c>
       <c r="C15" s="9">
+        <f t="shared" si="2"/>
+        <v>161</v>
+      </c>
+      <c r="D15" s="5" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>=B15+B14+B13</v>
+      </c>
+      <c r="F15" s="9">
+        <v>161</v>
+      </c>
+      <c r="G15" s="5"/>
+      <c r="I15" s="4">
+        <f t="shared" ca="1" si="4"/>
+        <v>161</v>
+      </c>
+      <c r="J15" s="4" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>=SUM(OFFSET(B15,-2,0,3))</v>
+      </c>
+      <c r="L15" s="8">
         <f t="shared" si="0"/>
         <v>161</v>
       </c>
-      <c r="D15" s="5" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>=B15+B14+B13</v>
-      </c>
-      <c r="F15" s="9">
+      <c r="M15" s="8" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>=SUM(B13:B15)</v>
+      </c>
+      <c r="O15" s="16">
+        <f t="shared" si="1"/>
         <v>161</v>
       </c>
-      <c r="G15" s="5"/>
-      <c r="I15" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>161</v>
-      </c>
-      <c r="J15" s="4" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>=SUM(OFFSET(B15,-2,0,3))</v>
-      </c>
-      <c r="L15" s="8">
-        <f>SUM(B13:B15)</f>
-        <v>161</v>
-      </c>
-      <c r="M15" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>=SUM(B13:B15)</v>
-      </c>
-      <c r="O15" s="16">
-        <f>_xlfn.AGGREGATE(9,4,B13:B15)</f>
-        <v>161</v>
-      </c>
       <c r="P15" s="16" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="7"/>
         <v>=AGGREGATE(9,4,B13:B15)</v>
       </c>
     </row>
@@ -2314,39 +2311,39 @@
         <v>10</v>
       </c>
       <c r="C16" s="9">
+        <f t="shared" si="2"/>
+        <v>85</v>
+      </c>
+      <c r="D16" s="5" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>=B16+B15+B14</v>
+      </c>
+      <c r="F16" s="9">
+        <v>85</v>
+      </c>
+      <c r="G16" s="5"/>
+      <c r="I16" s="4">
+        <f t="shared" ca="1" si="4"/>
+        <v>85</v>
+      </c>
+      <c r="J16" s="4" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>=SUM(OFFSET(B16,-2,0,3))</v>
+      </c>
+      <c r="L16" s="8">
         <f t="shared" si="0"/>
         <v>85</v>
       </c>
-      <c r="D16" s="5" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>=B16+B15+B14</v>
-      </c>
-      <c r="F16" s="9">
+      <c r="M16" s="8" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>=SUM(B14:B16)</v>
+      </c>
+      <c r="O16" s="16">
+        <f t="shared" si="1"/>
         <v>85</v>
       </c>
-      <c r="G16" s="5"/>
-      <c r="I16" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>85</v>
-      </c>
-      <c r="J16" s="4" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>=SUM(OFFSET(B16,-2,0,3))</v>
-      </c>
-      <c r="L16" s="8">
-        <f>SUM(B14:B16)</f>
-        <v>85</v>
-      </c>
-      <c r="M16" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>=SUM(B14:B16)</v>
-      </c>
-      <c r="O16" s="16">
-        <f>_xlfn.AGGREGATE(9,4,B14:B16)</f>
-        <v>85</v>
-      </c>
       <c r="P16" s="16" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="7"/>
         <v>=AGGREGATE(9,4,B14:B16)</v>
       </c>
     </row>
@@ -2355,39 +2352,39 @@
         <v>8</v>
       </c>
       <c r="C17" s="9">
+        <f t="shared" si="2"/>
+        <v>67</v>
+      </c>
+      <c r="D17" s="5" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>=B17+B16+B15</v>
+      </c>
+      <c r="F17" s="9">
+        <v>67</v>
+      </c>
+      <c r="G17" s="5"/>
+      <c r="I17" s="4">
+        <f t="shared" ca="1" si="4"/>
+        <v>67</v>
+      </c>
+      <c r="J17" s="4" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>=SUM(OFFSET(B17,-2,0,3))</v>
+      </c>
+      <c r="L17" s="8">
         <f t="shared" si="0"/>
         <v>67</v>
       </c>
-      <c r="D17" s="5" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>=B17+B16+B15</v>
-      </c>
-      <c r="F17" s="9">
+      <c r="M17" s="8" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>=SUM(B15:B17)</v>
+      </c>
+      <c r="O17" s="16">
+        <f t="shared" si="1"/>
         <v>67</v>
       </c>
-      <c r="G17" s="5"/>
-      <c r="I17" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>67</v>
-      </c>
-      <c r="J17" s="4" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>=SUM(OFFSET(B17,-2,0,3))</v>
-      </c>
-      <c r="L17" s="8">
-        <f>SUM(B15:B17)</f>
-        <v>67</v>
-      </c>
-      <c r="M17" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>=SUM(B15:B17)</v>
-      </c>
-      <c r="O17" s="16">
-        <f>_xlfn.AGGREGATE(9,4,B15:B17)</f>
-        <v>67</v>
-      </c>
       <c r="P17" s="16" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="7"/>
         <v>=AGGREGATE(9,4,B15:B17)</v>
       </c>
     </row>
@@ -2658,10 +2655,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73B545AF-F821-42A0-8F12-946DF16CC482}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:M39"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="O29" sqref="O29"/>
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2681,7 +2679,7 @@
         <v>16</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="17"/>
       <c r="F2" s="17"/>
@@ -2701,7 +2699,7 @@
         <v>17</v>
       </c>
       <c r="D3" s="23">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E3" s="17"/>
       <c r="F3" s="17"/>
@@ -2718,7 +2716,7 @@
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C4" s="22" t="str">
         <f>"Calculate the "&amp;UPPER($D$2)&amp;" over rolling windows of "&amp;D3&amp;" rows at a time"</f>
-        <v>Calculate the SUM over rolling windows of 3 rows at a time</v>
+        <v>Calculate the MIN over rolling windows of 9 rows at a time</v>
       </c>
       <c r="D4" s="21"/>
       <c r="E4" s="18"/>
@@ -2798,9 +2796,9 @@
       <c r="B8" s="6">
         <v>49</v>
       </c>
-      <c r="C8" s="24">
-        <f ca="1"/>
-        <v>195</v>
+      <c r="C8" s="24" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
       </c>
       <c r="D8" s="19"/>
       <c r="E8" s="18"/>
@@ -2819,9 +2817,9 @@
       <c r="B9" s="6">
         <v>72</v>
       </c>
-      <c r="C9" s="24">
-        <f ca="1"/>
-        <v>214</v>
+      <c r="C9" s="24" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="18"/>
@@ -2840,9 +2838,9 @@
       <c r="B10" s="6">
         <v>80</v>
       </c>
-      <c r="C10" s="24">
-        <f ca="1"/>
-        <v>201</v>
+      <c r="C10" s="24" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
       </c>
       <c r="D10" s="19"/>
       <c r="E10" s="18"/>
@@ -2861,9 +2859,9 @@
       <c r="B11" s="6">
         <v>79</v>
       </c>
-      <c r="C11" s="24">
-        <f ca="1"/>
-        <v>231</v>
+      <c r="C11" s="24" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
       </c>
       <c r="D11" s="19"/>
       <c r="E11" s="18"/>
@@ -2882,9 +2880,9 @@
       <c r="B12" s="6">
         <v>52</v>
       </c>
-      <c r="C12" s="24">
-        <f ca="1"/>
-        <v>211</v>
+      <c r="C12" s="24" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
       </c>
       <c r="D12" s="19"/>
       <c r="E12" s="18"/>
@@ -2903,9 +2901,9 @@
       <c r="B13" s="6">
         <v>46</v>
       </c>
-      <c r="C13" s="24">
-        <f ca="1"/>
-        <v>177</v>
+      <c r="C13" s="24" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
       </c>
       <c r="D13" s="19"/>
       <c r="E13" s="18"/>
@@ -2926,7 +2924,7 @@
       </c>
       <c r="C14" s="24">
         <f ca="1"/>
-        <v>184</v>
+        <v>46</v>
       </c>
       <c r="D14" s="19"/>
       <c r="E14" s="18"/>
@@ -2947,7 +2945,7 @@
       </c>
       <c r="C15" s="24">
         <f ca="1"/>
-        <v>158</v>
+        <v>26</v>
       </c>
       <c r="D15" s="19"/>
       <c r="E15" s="18"/>
@@ -2968,7 +2966,7 @@
       </c>
       <c r="C16" s="24">
         <f ca="1"/>
-        <v>161</v>
+        <v>26</v>
       </c>
       <c r="D16" s="19"/>
       <c r="E16" s="18"/>
@@ -2989,7 +2987,7 @@
       </c>
       <c r="C17" s="24">
         <f ca="1"/>
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="D17" s="19"/>
       <c r="E17" s="18"/>
@@ -3008,7 +3006,7 @@
       </c>
       <c r="C18" s="24">
         <f ca="1"/>
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="D18" s="19"/>
       <c r="E18" s="18"/>
@@ -3182,10 +3180,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67B85418-DF40-4528-B190-5955776B941F}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:T46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3208,13 +3207,13 @@
         <v>0</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E2" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="23" t="s">
         <v>6</v>
-      </c>
-      <c r="F2" s="23" t="s">
-        <v>5</v>
       </c>
       <c r="G2" s="17"/>
       <c r="H2" s="17"/>
@@ -3242,7 +3241,7 @@
         <v>6</v>
       </c>
       <c r="E3" s="23">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F3" s="23">
         <v>12</v>
@@ -3290,15 +3289,15 @@
       </c>
       <c r="D5" s="18" t="str" cm="1">
         <f t="array" ref="D5">IF(AND(D2="",D3=""),"","Rolling "&amp;UPPER(IF(D2="",_xlfn.LET(_xlpm.a,$C$2:$F$2,_xlpm.b,_xlfn._xlws.FILTER(_xlpm.a,_xlpm.a&lt;&gt;""),INDEX(_xlpm.b,1,COLUMNS(_xlpm.b))),D2))&amp;" of "&amp;IF(D3="",_xlfn.LET(_xlpm.a,$C$3:$F$3,_xlpm.b,_xlfn._xlws.FILTER(_xlpm.a,_xlpm.a&lt;&gt;""),INDEX(_xlpm.b,1,COLUMNS(_xlpm.b))),D3)&amp;" rows")</f>
-        <v>Rolling PRODUCT of 6 rows</v>
+        <v>Rolling SUM of 6 rows</v>
       </c>
       <c r="E5" s="18" t="str" cm="1">
         <f t="array" ref="E5">IF(AND(E2="",E3=""),"","Rolling "&amp;UPPER(IF(E2="",_xlfn.LET(_xlpm.a,$C$2:$F$2,_xlpm.b,_xlfn._xlws.FILTER(_xlpm.a,_xlpm.a&lt;&gt;""),INDEX(_xlpm.b,1,COLUMNS(_xlpm.b))),E2))&amp;" of "&amp;IF(E3="",_xlfn.LET(_xlpm.a,$C$3:$F$3,_xlpm.b,_xlfn._xlws.FILTER(_xlpm.a,_xlpm.a&lt;&gt;""),INDEX(_xlpm.b,1,COLUMNS(_xlpm.b))),E3)&amp;" rows")</f>
-        <v>Rolling SKEW of 9 rows</v>
+        <v>Rolling KURT of 4 rows</v>
       </c>
       <c r="F5" s="18" t="str" cm="1">
         <f t="array" ref="F5">IF(AND(F2="",F3=""),"","Rolling "&amp;UPPER(IF(F2="",_xlfn.LET(_xlpm.a,$C$2:$F$2,_xlpm.b,_xlfn._xlws.FILTER(_xlpm.a,_xlpm.a&lt;&gt;""),INDEX(_xlpm.b,1,COLUMNS(_xlpm.b))),F2))&amp;" of "&amp;IF(F3="",_xlfn.LET(_xlpm.a,$C$3:$F$3,_xlpm.b,_xlfn._xlws.FILTER(_xlpm.a,_xlpm.a&lt;&gt;""),INDEX(_xlpm.b,1,COLUMNS(_xlpm.b))),F3)&amp;" rows")</f>
-        <v>Rolling KURT of 12 rows</v>
+        <v>Rolling SKEW of 12 rows</v>
       </c>
       <c r="G5" s="18"/>
       <c r="H5" s="18"/>
@@ -3432,9 +3431,9 @@
         <f ca="1"/>
         <v>#N/A</v>
       </c>
-      <c r="E9" s="24" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
+      <c r="E9" s="24">
+        <f ca="1"/>
+        <v>-1.208428947383096</v>
       </c>
       <c r="F9" s="24" t="e">
         <f ca="1"/>
@@ -3467,9 +3466,9 @@
         <f ca="1"/>
         <v>#N/A</v>
       </c>
-      <c r="E10" s="24" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
+      <c r="E10" s="24">
+        <f ca="1"/>
+        <v>0.96796668649613338</v>
       </c>
       <c r="F10" s="24" t="e">
         <f ca="1"/>
@@ -3500,11 +3499,11 @@
       </c>
       <c r="D11" s="24">
         <f ca="1"/>
-        <v>109901715840</v>
-      </c>
-      <c r="E11" s="24" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
+        <v>426</v>
+      </c>
+      <c r="E11" s="24">
+        <f ca="1"/>
+        <v>2.6575090079514965</v>
       </c>
       <c r="F11" s="24" t="e">
         <f ca="1"/>
@@ -3535,11 +3534,11 @@
       </c>
       <c r="D12" s="24">
         <f ca="1"/>
-        <v>107828098560</v>
-      </c>
-      <c r="E12" s="24" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
+        <v>425</v>
+      </c>
+      <c r="E12" s="24">
+        <f ca="1"/>
+        <v>2.3357967877657551</v>
       </c>
       <c r="F12" s="24" t="e">
         <f ca="1"/>
@@ -3570,11 +3569,11 @@
       </c>
       <c r="D13" s="24">
         <f ca="1"/>
-        <v>53334328320</v>
-      </c>
-      <c r="E13" s="24" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
+        <v>378</v>
+      </c>
+      <c r="E13" s="24">
+        <f ca="1"/>
+        <v>-5.4238747676108012</v>
       </c>
       <c r="F13" s="24" t="e">
         <f ca="1"/>
@@ -3605,11 +3604,11 @@
       </c>
       <c r="D14" s="24">
         <f ca="1"/>
-        <v>93607188480</v>
+        <v>415</v>
       </c>
       <c r="E14" s="24">
         <f ca="1"/>
-        <v>3.6756906919595551E-2</v>
+        <v>-4.9450532774361466</v>
       </c>
       <c r="F14" s="24" t="e">
         <f ca="1"/>
@@ -3640,11 +3639,11 @@
       </c>
       <c r="D15" s="24">
         <f ca="1"/>
-        <v>33802595840</v>
+        <v>369</v>
       </c>
       <c r="E15" s="24">
         <f ca="1"/>
-        <v>-0.46156465853274181</v>
+        <v>1.5993268475759095</v>
       </c>
       <c r="F15" s="24" t="e">
         <f ca="1"/>
@@ -3675,11 +3674,11 @@
       </c>
       <c r="D16" s="24">
         <f ca="1"/>
-        <v>20704089952</v>
+        <v>338</v>
       </c>
       <c r="E16" s="24">
         <f ca="1"/>
-        <v>-0.19687836421155525</v>
+        <v>1.9751237551048817</v>
       </c>
       <c r="F16" s="24" t="e">
         <f ca="1"/>
@@ -3710,15 +3709,15 @@
       </c>
       <c r="D17" s="24">
         <f ca="1"/>
-        <v>2620770880</v>
+        <v>269</v>
       </c>
       <c r="E17" s="24">
         <f ca="1"/>
-        <v>-0.55647294088907795</v>
+        <v>-0.1714981267297464</v>
       </c>
       <c r="F17" s="24">
         <f ca="1"/>
-        <v>-0.36744715251425442</v>
+        <v>-0.40729879193182539</v>
       </c>
       <c r="G17" s="18"/>
       <c r="H17" s="18"/>
@@ -3745,15 +3744,15 @@
       </c>
       <c r="D18" s="24">
         <f ca="1"/>
-        <v>403195520</v>
+        <v>225</v>
       </c>
       <c r="E18" s="24">
         <f ca="1"/>
-        <v>-0.13314959171601332</v>
+        <v>2.4513372602786632E-2</v>
       </c>
       <c r="F18" s="24">
         <f ca="1"/>
-        <v>-1.0072916136984418</v>
+        <v>-0.35934308351838068</v>
       </c>
       <c r="G18" s="18"/>
       <c r="H18" s="18"/>

</xml_diff>